<commit_message>
cambios a los excel
</commit_message>
<xml_diff>
--- a/documentacion/Pert/PorFuncionalidad/pert_estimaciones_por_Funcionalidades.xlsx
+++ b/documentacion/Pert/PorFuncionalidad/pert_estimaciones_por_Funcionalidades.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaston\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6065B15E-4EB5-4065-96BE-3F95CBCADF98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B41FA1-8DEF-43F4-B8E2-92CD2ACE11D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Por Funcionalidad" sheetId="1" r:id="rId1"/>
-    <sheet name="Por Tareas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>Funcionalidad</t>
   </si>
@@ -121,52 +120,10 @@
     <t>mediana</t>
   </si>
   <si>
-    <t>Tarea</t>
-  </si>
-  <si>
-    <t>Diseño UI/UX</t>
-  </si>
-  <si>
-    <t>Configuración de proyectos</t>
-  </si>
-  <si>
-    <t>Autenticación y Roles</t>
-  </si>
-  <si>
-    <t>Gestión de Perfil</t>
-  </si>
-  <si>
-    <t>Gestión de Libros</t>
-  </si>
-  <si>
-    <t>Gestión de Reservas</t>
-  </si>
-  <si>
-    <t>Carrito de Compras</t>
-  </si>
-  <si>
-    <t>Favoritos</t>
-  </si>
-  <si>
-    <t>Reseñas y Comentarios</t>
-  </si>
-  <si>
-    <t>Reclamos y Bloqueos</t>
-  </si>
-  <si>
-    <t>Gestión de Novedades</t>
-  </si>
-  <si>
-    <t>Roles y Permisos</t>
-  </si>
-  <si>
-    <t>Integración Front-Back</t>
-  </si>
-  <si>
-    <t>Testing general</t>
-  </si>
-  <si>
     <t>SD</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -238,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -246,6 +203,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,9 +556,10 @@
     <col min="5" max="5" width="13.140625" customWidth="1"/>
     <col min="6" max="6" width="56.140625" customWidth="1"/>
     <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,10 +579,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -648,7 +610,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -673,7 +635,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -698,7 +660,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -723,7 +685,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -748,7 +710,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -773,7 +735,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -798,7 +760,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -823,7 +785,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -848,7 +810,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -873,7 +835,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -898,7 +860,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -923,7 +885,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -948,7 +910,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -973,7 +935,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -998,7 +960,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1023,7 +985,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1048,7 +1010,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1073,7 +1035,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1098,7 +1060,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1121,423 +1083,31 @@
       <c r="G21">
         <f t="shared" si="0"/>
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23">
+        <f>SUM(F2:F21)</f>
+        <v>42.833333333333329</v>
+      </c>
+      <c r="G23">
+        <f>SUM(G2:G21)</f>
+        <v>8.5</v>
+      </c>
+      <c r="H23">
+        <f>SUM(F23:G23)</f>
+        <v>51.333333333333329</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <v>2.166666666666667</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3">
-        <v>0.5</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1.083333333333333</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>3.166666666666667</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>3.166666666666667</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>2.166666666666667</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>3.166666666666667</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>4</v>
-      </c>
-      <c r="F8">
-        <v>2.166666666666667</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9">
-        <v>0.5</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>1.083333333333333</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10">
-        <v>0.5</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="F10">
-        <v>1.083333333333333</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11">
-        <v>4</v>
-      </c>
-      <c r="F11">
-        <v>2.166666666666667</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <v>4</v>
-      </c>
-      <c r="F12">
-        <v>2.166666666666667</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-      <c r="E13">
-        <v>5</v>
-      </c>
-      <c r="F13">
-        <v>3.166666666666667</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14">
-        <v>0.5</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
-      <c r="F14">
-        <v>1.083333333333333</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
-      <c r="E15">
-        <v>5</v>
-      </c>
-      <c r="F15">
-        <v>3.166666666666667</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-      <c r="E16">
-        <v>4</v>
-      </c>
-      <c r="F16">
-        <v>2.166666666666667</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17">
-        <v>3</v>
-      </c>
-      <c r="E17">
-        <v>5</v>
-      </c>
-      <c r="F17">
-        <v>3.166666666666667</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18">
-        <v>3</v>
-      </c>
-      <c r="E18">
-        <v>5</v>
-      </c>
-      <c r="F18">
-        <v>3.166666666666667</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>2</v>
-      </c>
-      <c r="E19">
-        <v>4</v>
-      </c>
-      <c r="F19">
-        <v>2.166666666666667</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>2</v>
-      </c>
-      <c r="E20">
-        <v>4</v>
-      </c>
-      <c r="F20">
-        <v>2.166666666666667</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>